<commit_message>
Refractored some code. Improved address splitting algorithm.
Moved some code from the main to their specific classes. Also streamlined the generation of xmls from a single excel.
</commit_message>
<xml_diff>
--- a/TiaAddin-Spin-ExcelReader/Templates/Q4A-1.xlsx
+++ b/TiaAddin-Spin-ExcelReader/Templates/Q4A-1.xlsx
@@ -1,13 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zanetti r\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PARONETTO G\Documents\GitHub\TiaAddIn-Spin\TiaAddin-Spin-ExcelReader\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7232588E-8996-42B4-835E-A3E0F4B85929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BIT" sheetId="1" r:id="rId1"/>
@@ -15,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BIT!$A$1:$T$70</definedName>
   </definedNames>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="178">
   <si>
     <t>Indirizzo</t>
   </si>
@@ -559,8 +562,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -588,7 +591,13 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -600,10 +609,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -612,10 +629,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -891,39 +908,44 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.71094" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.855469" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.425781" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.71094" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85547" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.57031" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85547" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.14063" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.570313" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.710938" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.42578" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.285156" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.14063" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.71094" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.71094" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -985,9 +1007,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>21</v>
@@ -1047,9 +1069,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
@@ -1109,7 +1131,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
@@ -1171,7 +1193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>40</v>
       </c>
@@ -1233,7 +1255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
@@ -1295,7 +1317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
@@ -1357,7 +1379,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
@@ -1419,7 +1441,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
@@ -1481,7 +1503,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>56</v>
       </c>
@@ -1543,7 +1565,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>61</v>
       </c>
@@ -1605,7 +1627,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>63</v>
       </c>
@@ -1667,7 +1689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>66</v>
       </c>
@@ -1729,7 +1751,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>70</v>
       </c>
@@ -1791,7 +1813,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>73</v>
       </c>
@@ -1853,7 +1875,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>76</v>
       </c>
@@ -1915,7 +1937,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>79</v>
       </c>
@@ -1977,7 +1999,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -2039,7 +2061,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>85</v>
       </c>
@@ -2101,7 +2123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>90</v>
       </c>
@@ -2163,7 +2185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>93</v>
       </c>
@@ -2225,7 +2247,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>95</v>
       </c>
@@ -2287,7 +2309,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>96</v>
       </c>
@@ -2349,7 +2371,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>97</v>
       </c>
@@ -2411,7 +2433,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>99</v>
       </c>
@@ -2473,7 +2495,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>101</v>
       </c>
@@ -2535,7 +2557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>103</v>
       </c>
@@ -2597,7 +2619,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>106</v>
       </c>
@@ -2659,7 +2681,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>110</v>
       </c>
@@ -2721,7 +2743,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>112</v>
       </c>
@@ -2783,7 +2805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>113</v>
       </c>
@@ -2845,7 +2867,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>114</v>
       </c>
@@ -2907,7 +2929,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>115</v>
       </c>
@@ -2969,7 +2991,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>116</v>
       </c>
@@ -3031,7 +3053,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
@@ -3093,7 +3115,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>117</v>
       </c>
@@ -3155,7 +3177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>122</v>
       </c>
@@ -3217,7 +3239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>123</v>
       </c>
@@ -3279,7 +3301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>124</v>
       </c>
@@ -3341,7 +3363,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>125</v>
       </c>
@@ -3403,7 +3425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>126</v>
       </c>
@@ -3465,7 +3487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>127</v>
       </c>
@@ -3527,7 +3549,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>128</v>
       </c>
@@ -3589,7 +3611,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>130</v>
       </c>
@@ -3651,7 +3673,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>132</v>
       </c>
@@ -3713,7 +3735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>134</v>
       </c>
@@ -3775,7 +3797,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>135</v>
       </c>
@@ -3837,7 +3859,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>136</v>
       </c>
@@ -3899,7 +3921,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>137</v>
       </c>
@@ -3961,7 +3983,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>138</v>
       </c>
@@ -4023,7 +4045,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>139</v>
       </c>
@@ -4085,7 +4107,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>26</v>
       </c>
@@ -4147,7 +4169,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>142</v>
       </c>
@@ -4209,7 +4231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>150</v>
       </c>
@@ -4271,7 +4293,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>152</v>
       </c>
@@ -4333,7 +4355,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>156</v>
       </c>
@@ -4395,7 +4417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>158</v>
       </c>
@@ -4457,7 +4479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>160</v>
       </c>
@@ -4519,7 +4541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>162</v>
       </c>
@@ -4581,7 +4603,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>164</v>
       </c>
@@ -4643,7 +4665,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>26</v>
       </c>
@@ -4705,7 +4727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>166</v>
       </c>
@@ -4767,7 +4789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>171</v>
       </c>
@@ -4829,7 +4851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>172</v>
       </c>
@@ -4891,7 +4913,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>173</v>
       </c>
@@ -4953,7 +4975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>174</v>
       </c>
@@ -5015,7 +5037,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>175</v>
       </c>
@@ -5077,7 +5099,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>176</v>
       </c>
@@ -5139,7 +5161,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>177</v>
       </c>
@@ -5201,7 +5223,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>26</v>
       </c>
@@ -5264,6 +5286,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T70"/>
+  <autoFilter ref="A1:T70" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>